<commit_message>
Add Practical Session  in one PDF
</commit_message>
<xml_diff>
--- a/DGE_CRED_Model/ExcelFiles/Data/Damages.xlsx
+++ b/DGE_CRED_Model/ExcelFiles/Data/Damages.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_9BB35308C023412BD391EE68BFFE6B70BA26F412" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C189739A-FBD4-44C9-97BD-BFA019338391}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rice and Agriculture" sheetId="3" r:id="rId1"/>
@@ -12,17 +13,26 @@
     <sheet name="Construction" sheetId="5" r:id="rId3"/>
     <sheet name="Transport" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="58">
   <si>
     <t>SLR</t>
   </si>
@@ -192,11 +202,17 @@
   <si>
     <t>0.0125785296317374+VLOOKUP(</t>
   </si>
+  <si>
+    <t>Cumulative Vietnam</t>
+  </si>
+  <si>
+    <t>cum.Vietnam</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,7 +552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1799,7 +1815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:V15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2514,11 +2530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3208,7 +3224,7 @@
         <v>49324606.921025135</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>65</v>
       </c>
@@ -3255,7 +3271,7 @@
         <v>42335765.488584489</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>70</v>
       </c>
@@ -3302,7 +3318,7 @@
         <v>55357227.174870551</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>75</v>
       </c>
@@ -3349,7 +3365,7 @@
         <v>50501512.804503359</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>80</v>
       </c>
@@ -3396,7 +3412,7 @@
         <v>50635167.507927999</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>85</v>
       </c>
@@ -3443,7 +3459,7 @@
         <v>41673042.9420892</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>90</v>
       </c>
@@ -3490,7 +3506,7 @@
         <v>37098445.351677507</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>95</v>
       </c>
@@ -3537,7 +3553,7 @@
         <v>35217596.47064846</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3545,7 +3561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -3591,8 +3607,11 @@
       <c r="O25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3638,8 +3657,12 @@
       <c r="O26">
         <v>4.4578871888420477E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P26">
+        <f>O26</f>
+        <v>4.4578871888420477E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>5</v>
       </c>
@@ -3685,8 +3708,12 @@
       <c r="O27">
         <v>3.7219198423985339E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P27">
+        <f t="shared" ref="P27:P45" si="0">O27+P26</f>
+        <v>8.179807031240582E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>10</v>
       </c>
@@ -3732,8 +3759,12 @@
       <c r="O28">
         <v>1.1044104369819585E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>1.9223911401060167E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>15</v>
       </c>
@@ -3779,8 +3810,12 @@
       <c r="O29">
         <v>1.0703057519275676E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>2.9926968920335844E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>20</v>
       </c>
@@ -3826,8 +3861,12 @@
       <c r="O30">
         <v>2.0826848798903265E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>5.0753817719239105E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>25</v>
       </c>
@@ -3873,8 +3912,12 @@
       <c r="O31">
         <v>2.5467313182140432E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>5.3300549037453147E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3919,6 +3962,10 @@
       </c>
       <c r="O32">
         <v>3.9539181928540546E-3</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>5.72544672303072E-2</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -3967,6 +4014,10 @@
       <c r="O33">
         <v>4.2967783566585562E-3</v>
       </c>
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>6.1551245586965758E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
@@ -4014,6 +4065,10 @@
       <c r="O34">
         <v>6.4333795522697962E-3</v>
       </c>
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>6.798462513923556E-2</v>
+      </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
@@ -4061,6 +4116,10 @@
       <c r="O35">
         <v>7.8068157558490968E-3</v>
       </c>
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>7.5791440895084661E-2</v>
+      </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
@@ -4108,6 +4167,10 @@
       <c r="O36">
         <v>1.1469990980547804E-2</v>
       </c>
+      <c r="P36">
+        <f t="shared" si="0"/>
+        <v>8.726143187563247E-2</v>
+      </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
@@ -4155,6 +4218,10 @@
       <c r="O37">
         <v>1.235537219632328E-2</v>
       </c>
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>9.961680407195575E-2</v>
+      </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
@@ -4202,6 +4269,10 @@
       <c r="O38">
         <v>1.1652576946137487E-2</v>
       </c>
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>0.11126938101809324</v>
+      </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
@@ -4249,6 +4320,10 @@
       <c r="O39">
         <v>1.0001514370286435E-2</v>
       </c>
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>0.12127089538837967</v>
+      </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
@@ -4296,6 +4371,10 @@
       <c r="O40">
         <v>1.3077739275506135E-2</v>
       </c>
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>0.1343486346638858</v>
+      </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
@@ -4343,6 +4422,10 @@
       <c r="O41">
         <v>1.1930612337023616E-2</v>
       </c>
+      <c r="P41">
+        <f t="shared" si="0"/>
+        <v>0.14627924700090941</v>
+      </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
@@ -4390,6 +4473,10 @@
       <c r="O42">
         <v>1.19621872813179E-2</v>
       </c>
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>0.15824143428222731</v>
+      </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
@@ -4437,6 +4524,10 @@
       <c r="O43">
         <v>9.8449510249496719E-3</v>
       </c>
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>0.16808638530717698</v>
+      </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
@@ -4484,6 +4575,10 @@
       <c r="O44">
         <v>8.7642358657749279E-3</v>
       </c>
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>0.17685062117295192</v>
+      </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
@@ -4530,6 +4625,10 @@
       </c>
       <c r="O45">
         <v>8.3198991000437983E-3</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>0.18517052027299571</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -6566,11 +6665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W212"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="O105" sqref="O105"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7176,7 +7275,7 @@
         <v>98114728.30550459</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>65</v>
       </c>
@@ -7217,7 +7316,7 @@
         <v>91727658.23635444</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>70</v>
       </c>
@@ -7258,7 +7357,7 @@
         <v>100422861.71232937</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>75</v>
       </c>
@@ -7299,7 +7398,7 @@
         <v>96285150.381826103</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>80</v>
       </c>
@@ -7340,7 +7439,7 @@
         <v>124363366.34188136</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>85</v>
       </c>
@@ -7381,7 +7480,7 @@
         <v>110146248.17967762</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>90</v>
       </c>
@@ -7422,7 +7521,7 @@
         <v>109005177.01970309</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>95</v>
       </c>
@@ -7463,7 +7562,7 @@
         <v>184572179.41156667</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -7471,7 +7570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -7509,7 +7608,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -7555,8 +7654,11 @@
       <c r="O26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>0</v>
       </c>
@@ -7602,8 +7704,12 @@
       <c r="O27">
         <v>1.1388796132961147E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P27">
+        <f>O27</f>
+        <v>1.1388796132961147E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>5</v>
       </c>
@@ -7649,8 +7755,12 @@
       <c r="O28">
         <v>1.0942243501945826E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P28">
+        <f>P27+O28</f>
+        <v>2.2331039634906971E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>10</v>
       </c>
@@ -7696,8 +7806,12 @@
       <c r="O29">
         <v>2.3386825242349894E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P29">
+        <f t="shared" ref="P29:P46" si="0">P28+O29</f>
+        <v>4.5717864877256861E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>15</v>
       </c>
@@ -7743,8 +7857,12 @@
       <c r="O30">
         <v>2.4513946274128041E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>7.023181115138491E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>20</v>
       </c>
@@ -7790,8 +7908,12 @@
       <c r="O31">
         <v>3.8548163945216478E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>0.10877997509660139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>25</v>
       </c>
@@ -7836,6 +7958,10 @@
       </c>
       <c r="O32">
         <v>1.119897713357198E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>0.11997895223017338</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -7884,6 +8010,10 @@
       <c r="O33">
         <v>1.550634965514793E-2</v>
       </c>
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>0.13548530188532132</v>
+      </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
@@ -7931,6 +8061,10 @@
       <c r="O34">
         <v>1.2371911991887273E-2</v>
       </c>
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>0.1478572138772086</v>
+      </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
@@ -7978,6 +8112,10 @@
       <c r="O35">
         <v>1.7391141134408612E-2</v>
       </c>
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>0.16524835501161722</v>
+      </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
@@ -8025,6 +8163,10 @@
       <c r="O36">
         <v>2.0246722957205931E-2</v>
       </c>
+      <c r="P36">
+        <f t="shared" si="0"/>
+        <v>0.18549507796882314</v>
+      </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
@@ -8072,6 +8214,10 @@
       <c r="O37">
         <v>2.0561179839098404E-2</v>
       </c>
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>0.20605625780792156</v>
+      </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
@@ -8119,6 +8265,10 @@
       <c r="O38">
         <v>1.9137742880632712E-2</v>
       </c>
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>0.22519400068855427</v>
+      </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
@@ -8166,6 +8316,10 @@
       <c r="O39">
         <v>2.3178885600848586E-2</v>
       </c>
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>0.24837288628940285</v>
+      </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
@@ -8213,6 +8367,10 @@
       <c r="O40">
         <v>2.1669987099937893E-2</v>
       </c>
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>0.27004287338934074</v>
+      </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
@@ -8260,6 +8418,10 @@
       <c r="O41">
         <v>2.372416520475986E-2</v>
       </c>
+      <c r="P41">
+        <f t="shared" si="0"/>
+        <v>0.29376703859410058</v>
+      </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
@@ -8307,6 +8469,10 @@
       <c r="O42">
         <v>2.2746661223090173E-2</v>
       </c>
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>0.31651369981719074</v>
+      </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
@@ -8354,6 +8520,10 @@
       <c r="O43">
         <v>2.9379933993183841E-2</v>
       </c>
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>0.34589363381037458</v>
+      </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
@@ -8401,6 +8571,10 @@
       <c r="O44">
         <v>2.6021244007014055E-2</v>
       </c>
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>0.37191487781738863</v>
+      </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
@@ -8448,6 +8622,10 @@
       <c r="O45">
         <v>2.575167430696737E-2</v>
       </c>
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>0.39766655212435598</v>
+      </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
@@ -8494,6 +8672,10 @@
       </c>
       <c r="O46">
         <v>4.360382488507572E-2</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="0"/>
+        <v>0.44127037700943172</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="25.8" x14ac:dyDescent="0.95">

</xml_diff>